<commit_message>
update results with correct trial number
</commit_message>
<xml_diff>
--- a/results-within.xlsx
+++ b/results-within.xlsx
@@ -433,7 +433,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -444,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -455,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -466,7 +466,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -477,7 +477,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -488,7 +488,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -510,10 +510,10 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -521,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -532,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -543,7 +543,7 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -554,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -565,7 +565,7 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -576,7 +576,7 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -587,7 +587,7 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -598,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -609,7 +609,7 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -620,7 +620,7 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -631,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -642,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -653,7 +653,7 @@
         <v>3</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -664,7 +664,7 @@
         <v>3</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -675,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -686,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -697,7 +697,7 @@
         <v>3</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -708,7 +708,7 @@
         <v>3</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -719,7 +719,7 @@
         <v>3</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -730,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -741,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -752,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -774,7 +774,7 @@
         <v>3</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -785,7 +785,7 @@
         <v>3</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -796,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -807,7 +807,7 @@
         <v>3</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -818,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -829,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -840,7 +840,7 @@
         <v>3</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -851,7 +851,7 @@
         <v>3</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -862,7 +862,7 @@
         <v>3</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -897,7 +897,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -908,7 +908,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -919,7 +919,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -930,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -941,7 +941,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -952,7 +952,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -963,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -974,7 +974,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -985,7 +985,7 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -996,7 +996,7 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1007,7 +1007,7 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1029,7 +1029,7 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1040,7 +1040,7 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1051,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1062,7 +1062,7 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1073,7 +1073,7 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1084,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1095,7 +1095,7 @@
         <v>4</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1106,7 +1106,7 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1117,7 +1117,7 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1128,7 +1128,7 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1139,7 +1139,7 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1150,7 +1150,7 @@
         <v>4</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1161,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1172,7 +1172,7 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1183,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1194,7 +1194,7 @@
         <v>4</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1205,7 +1205,7 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1216,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1227,7 +1227,7 @@
         <v>4</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1238,7 +1238,7 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1249,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1260,7 +1260,7 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1271,7 +1271,7 @@
         <v>4</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1282,7 +1282,7 @@
         <v>4</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -1293,7 +1293,7 @@
         <v>4</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1304,7 +1304,7 @@
         <v>4</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1315,7 +1315,7 @@
         <v>4</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1326,7 +1326,7 @@
         <v>4</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1361,7 +1361,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1372,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1383,7 +1383,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1394,7 +1394,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1405,7 +1405,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1416,7 +1416,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1427,7 +1427,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1438,7 +1438,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1449,7 +1449,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1460,7 +1460,7 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1471,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1482,7 +1482,7 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1493,7 +1493,7 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1504,7 +1504,7 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1515,7 +1515,7 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1526,7 +1526,7 @@
         <v>5</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1537,7 +1537,7 @@
         <v>5</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1548,7 +1548,7 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1559,7 +1559,7 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1570,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1581,7 +1581,7 @@
         <v>5</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1592,7 +1592,7 @@
         <v>5</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1603,7 +1603,7 @@
         <v>5</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1614,7 +1614,7 @@
         <v>5</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1625,7 +1625,7 @@
         <v>5</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1636,7 +1636,7 @@
         <v>5</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1647,7 +1647,7 @@
         <v>5</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1658,7 +1658,7 @@
         <v>5</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1669,7 +1669,7 @@
         <v>5</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1680,7 +1680,7 @@
         <v>5</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1691,7 +1691,7 @@
         <v>5</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1702,7 +1702,7 @@
         <v>5</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1713,7 +1713,7 @@
         <v>5</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1724,7 +1724,7 @@
         <v>5</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1735,7 +1735,7 @@
         <v>5</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1746,7 +1746,7 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1757,7 +1757,7 @@
         <v>5</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1768,7 +1768,7 @@
         <v>5</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1779,7 +1779,7 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1790,7 +1790,7 @@
         <v>5</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1825,7 +1825,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1836,7 +1836,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1847,7 +1847,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1858,7 +1858,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1869,7 +1869,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1880,7 +1880,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1891,7 +1891,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1902,7 +1902,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1913,7 +1913,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1924,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1935,7 +1935,7 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1946,7 +1946,7 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1957,7 +1957,7 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1968,7 +1968,7 @@
         <v>6</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1979,7 +1979,7 @@
         <v>6</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1990,7 +1990,7 @@
         <v>6</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2001,7 +2001,7 @@
         <v>6</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2012,7 +2012,7 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2023,7 +2023,7 @@
         <v>6</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2034,7 +2034,7 @@
         <v>6</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2045,7 +2045,7 @@
         <v>6</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -2056,7 +2056,7 @@
         <v>6</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2067,7 +2067,7 @@
         <v>6</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -2078,7 +2078,7 @@
         <v>6</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -2089,7 +2089,7 @@
         <v>6</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2100,7 +2100,7 @@
         <v>6</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -2111,7 +2111,7 @@
         <v>6</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2122,7 +2122,7 @@
         <v>6</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2133,7 +2133,7 @@
         <v>6</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -2144,7 +2144,7 @@
         <v>6</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -2155,7 +2155,7 @@
         <v>6</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2166,7 +2166,7 @@
         <v>6</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2177,7 +2177,7 @@
         <v>6</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2188,7 +2188,7 @@
         <v>6</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -2199,7 +2199,7 @@
         <v>6</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -2210,7 +2210,7 @@
         <v>6</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2221,7 +2221,7 @@
         <v>6</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2232,7 +2232,7 @@
         <v>6</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2243,7 +2243,7 @@
         <v>6</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2254,7 +2254,7 @@
         <v>6</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2289,7 +2289,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -2300,7 +2300,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2311,7 +2311,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2322,7 +2322,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2333,7 +2333,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2344,7 +2344,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2355,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2366,7 +2366,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2377,7 +2377,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2388,7 +2388,7 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2399,7 +2399,7 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2410,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2421,7 +2421,7 @@
         <v>7</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2432,7 +2432,7 @@
         <v>7</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2443,7 +2443,7 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2454,7 +2454,7 @@
         <v>7</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2465,7 +2465,7 @@
         <v>7</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -2476,7 +2476,7 @@
         <v>7</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2487,7 +2487,7 @@
         <v>7</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2498,7 +2498,7 @@
         <v>7</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2509,7 +2509,7 @@
         <v>7</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2520,7 +2520,7 @@
         <v>7</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2531,7 +2531,7 @@
         <v>7</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2542,7 +2542,7 @@
         <v>7</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2553,7 +2553,7 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2564,7 +2564,7 @@
         <v>7</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2575,7 +2575,7 @@
         <v>7</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2586,7 +2586,7 @@
         <v>7</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2597,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -2608,7 +2608,7 @@
         <v>7</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -2619,7 +2619,7 @@
         <v>7</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2630,7 +2630,7 @@
         <v>7</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -2641,7 +2641,7 @@
         <v>7</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2652,7 +2652,7 @@
         <v>7</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -2663,7 +2663,7 @@
         <v>7</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2674,7 +2674,7 @@
         <v>7</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -2685,7 +2685,7 @@
         <v>7</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2696,7 +2696,7 @@
         <v>7</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -2707,7 +2707,7 @@
         <v>7</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -2718,7 +2718,7 @@
         <v>7</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -2753,7 +2753,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2764,7 +2764,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2775,7 +2775,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2786,7 +2786,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2797,7 +2797,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2808,7 +2808,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2819,7 +2819,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2830,7 +2830,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2841,7 +2841,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2852,7 +2852,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2863,7 +2863,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2874,7 +2874,7 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2896,7 +2896,7 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -2907,7 +2907,7 @@
         <v>8</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -2918,7 +2918,7 @@
         <v>8</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2929,7 +2929,7 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2940,7 +2940,7 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -2951,7 +2951,7 @@
         <v>8</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2962,7 +2962,7 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2973,7 +2973,7 @@
         <v>8</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2984,7 +2984,7 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2995,7 +2995,7 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3006,7 +3006,7 @@
         <v>8</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3017,7 +3017,7 @@
         <v>8</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3028,7 +3028,7 @@
         <v>8</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -3039,7 +3039,7 @@
         <v>8</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -3050,7 +3050,7 @@
         <v>8</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3061,7 +3061,7 @@
         <v>8</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -3072,7 +3072,7 @@
         <v>8</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3083,7 +3083,7 @@
         <v>8</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3094,7 +3094,7 @@
         <v>8</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3105,7 +3105,7 @@
         <v>8</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -3116,7 +3116,7 @@
         <v>8</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3127,7 +3127,7 @@
         <v>8</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3138,7 +3138,7 @@
         <v>8</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -3149,7 +3149,7 @@
         <v>8</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -3160,7 +3160,7 @@
         <v>8</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -3171,7 +3171,7 @@
         <v>8</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -3182,7 +3182,7 @@
         <v>8</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -3217,10 +3217,10 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3228,7 +3228,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3239,7 +3239,7 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -3250,7 +3250,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -3261,7 +3261,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3272,7 +3272,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -3283,7 +3283,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -3294,7 +3294,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -3305,7 +3305,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -3316,7 +3316,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -3327,7 +3327,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -3338,7 +3338,7 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -3349,7 +3349,7 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -3360,7 +3360,7 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3371,7 +3371,7 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3382,7 +3382,7 @@
         <v>9</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -3393,7 +3393,7 @@
         <v>9</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3404,7 +3404,7 @@
         <v>9</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -3415,7 +3415,7 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3426,7 +3426,7 @@
         <v>9</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -3437,7 +3437,7 @@
         <v>9</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3448,7 +3448,7 @@
         <v>9</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3459,7 +3459,7 @@
         <v>9</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3470,7 +3470,7 @@
         <v>9</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3481,7 +3481,7 @@
         <v>9</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3492,7 +3492,7 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3503,7 +3503,7 @@
         <v>9</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3514,7 +3514,7 @@
         <v>9</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3525,7 +3525,7 @@
         <v>9</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3536,7 +3536,7 @@
         <v>9</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3547,7 +3547,7 @@
         <v>9</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3558,7 +3558,7 @@
         <v>9</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3569,7 +3569,7 @@
         <v>9</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3580,7 +3580,7 @@
         <v>9</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3591,7 +3591,7 @@
         <v>9</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3602,7 +3602,7 @@
         <v>9</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3613,7 +3613,7 @@
         <v>9</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -3624,7 +3624,7 @@
         <v>9</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -3635,7 +3635,7 @@
         <v>9</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3646,7 +3646,7 @@
         <v>9</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3681,7 +3681,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -3692,7 +3692,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3703,7 +3703,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3714,7 +3714,7 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3725,7 +3725,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3736,7 +3736,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -3747,7 +3747,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -3758,7 +3758,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -3769,7 +3769,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -3780,7 +3780,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3791,7 +3791,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3802,7 +3802,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -3813,7 +3813,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -3824,7 +3824,7 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3835,7 +3835,7 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3846,7 +3846,7 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3857,7 +3857,7 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -3868,7 +3868,7 @@
         <v>10</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -3879,7 +3879,7 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3890,7 +3890,7 @@
         <v>10</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -3901,7 +3901,7 @@
         <v>10</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -3912,7 +3912,7 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3923,7 +3923,7 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3934,7 +3934,7 @@
         <v>10</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3945,10 +3945,10 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3956,7 +3956,7 @@
         <v>10</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3967,7 +3967,7 @@
         <v>10</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3978,7 +3978,7 @@
         <v>10</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3989,7 +3989,7 @@
         <v>10</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -4000,7 +4000,7 @@
         <v>10</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -4011,7 +4011,7 @@
         <v>10</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -4022,7 +4022,7 @@
         <v>10</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -4033,7 +4033,7 @@
         <v>10</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -4044,7 +4044,7 @@
         <v>10</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -4055,7 +4055,7 @@
         <v>10</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -4066,7 +4066,7 @@
         <v>10</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -4077,7 +4077,7 @@
         <v>10</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -4088,7 +4088,7 @@
         <v>10</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -4099,7 +4099,7 @@
         <v>10</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -4110,7 +4110,7 @@
         <v>10</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>1</v>

</xml_diff>